<commit_message>
Update research paper graphs.xlsx
</commit_message>
<xml_diff>
--- a/Research paper/research paper graphs.xlsx
+++ b/Research paper/research paper graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New folder\Major_project\Research paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20832D5C-2013-459B-A25E-AD814D81C6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE529F8B-FD5F-41F9-83B2-05FD4EA3EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{E6209FDB-AA24-4EEE-BF2D-9978D18E9C37}"/>
+    <workbookView xWindow="2730" yWindow="315" windowWidth="21600" windowHeight="11385" xr2:uid="{E6209FDB-AA24-4EEE-BF2D-9978D18E9C37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>year</t>
   </si>
@@ -55,6 +46,21 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Countries</t>
   </si>
 </sst>
 </file>
@@ -163,6 +169,15 @@
             <a:r>
               <a:rPr lang="en-IN" baseline="0"/>
               <a:t> Comparison</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t>(in Billions)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -630,7 +645,564 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Penetration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> Comparison</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t>(by %)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Qatar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>US</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$24:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3144-4AAF-AD61-E4B63A3AC8D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Qatar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>US</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$25:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>82.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3144-4AAF-AD61-E4B63A3AC8D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Qatar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>US</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$26:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>86.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3144-4AAF-AD61-E4B63A3AC8D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="811731088"/>
+        <c:axId val="838222912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="811731088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="838222912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="838222912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="811731088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1173,6 +1745,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1206,6 +2281,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F3927D-3E88-15B1-0785-030E3E788FB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1511,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A660162B-1D06-42E8-93BC-B1BD7C90E1F2}">
-  <dimension ref="B2:G13"/>
+  <dimension ref="B2:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,6 +2742,170 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2021</v>
+      </c>
+      <c r="C24">
+        <v>74.8</v>
+      </c>
+      <c r="D24">
+        <v>70.2</v>
+      </c>
+      <c r="E24">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F24">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G24">
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2022</v>
+      </c>
+      <c r="C25">
+        <v>82.2</v>
+      </c>
+      <c r="D25">
+        <v>77.3</v>
+      </c>
+      <c r="E25">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="F25">
+        <v>75.2</v>
+      </c>
+      <c r="G25">
+        <v>75.2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2023</v>
+      </c>
+      <c r="C26">
+        <v>86.8</v>
+      </c>
+      <c r="D26">
+        <v>82.1</v>
+      </c>
+      <c r="E26">
+        <v>80.5</v>
+      </c>
+      <c r="F26">
+        <v>80.5</v>
+      </c>
+      <c r="G26">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>2021</v>
+      </c>
+      <c r="D37">
+        <v>2022</v>
+      </c>
+      <c r="E37">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>74.8</v>
+      </c>
+      <c r="D38">
+        <v>82.2</v>
+      </c>
+      <c r="E38">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>70.2</v>
+      </c>
+      <c r="D39">
+        <v>77.3</v>
+      </c>
+      <c r="E39">
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="D40">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="E40">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="D41">
+        <v>75.2</v>
+      </c>
+      <c r="E41">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>68.3</v>
+      </c>
+      <c r="D42">
+        <v>75.2</v>
+      </c>
+      <c r="E42">
+        <v>79.8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" display="https://www.marketsandmarkets.com/Market-Reports/virtual-classroom-market-203811025.html" xr:uid="{57FB342B-4E6E-490D-A639-015A8D67E0EE}"/>

</xml_diff>